<commit_message>
Added Java ForkJoin impl.
</commit_message>
<xml_diff>
--- a/doc/results.xlsx
+++ b/doc/results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhurst/dev/nqueens/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB9CF8A-56FE-A74C-AB9B-C070EE52345A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30480" yWindow="680" windowWidth="28040" windowHeight="17440" xr2:uid="{914555B8-60BB-8E47-AB9E-7A25BB291EE9}"/>
+    <workbookView xWindow="21180" yWindow="680" windowWidth="17220" windowHeight="17440" xr2:uid="{914555B8-60BB-8E47-AB9E-7A25BB291EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Macbook Pro 2016" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Version</t>
   </si>
@@ -96,6 +97,9 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>JaaForkJoin-2</t>
   </si>
 </sst>
 </file>
@@ -447,13 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240F3C8E-C1A7-294F-8537-256A32EA6A43}">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -885,213 +889,236 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D19">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="E19">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="F19">
-        <v>0.192</v>
+        <v>24</v>
       </c>
       <c r="G19">
-        <v>1.1519999999999999</v>
+        <v>0.83</v>
       </c>
       <c r="H19">
-        <v>4.8929999999999998</v>
+        <v>0.41</v>
       </c>
       <c r="I19">
-        <v>27.4</v>
+        <v>2.8359999999999999</v>
       </c>
       <c r="J19">
-        <v>188</v>
+        <v>19.347000000000001</v>
       </c>
       <c r="K19">
-        <v>1355</v>
+        <v>138</v>
+      </c>
+      <c r="L19">
+        <v>1042</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D20">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E20">
-        <v>7.4999999999999997E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F20">
-        <v>7.3999999999999996E-2</v>
+        <v>0.192</v>
       </c>
       <c r="G20">
-        <v>0.35199999999999998</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="H20">
-        <v>1.5449999999999999</v>
+        <v>4.8929999999999998</v>
       </c>
       <c r="I20">
-        <v>8.1999999999999993</v>
+        <v>27.4</v>
       </c>
       <c r="J20">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="K20">
-        <v>682</v>
-      </c>
-      <c r="L20">
-        <v>3228</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D21">
-        <v>3.0000000000000001E-3</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E21">
-        <v>1.4E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F21">
-        <v>8.3000000000000004E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="G21">
-        <v>0.434</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="H21">
-        <v>2.7090000000000001</v>
+        <v>1.5449999999999999</v>
       </c>
       <c r="I21">
-        <v>16.899999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="J21">
-        <v>115</v>
+        <v>56</v>
+      </c>
+      <c r="K21">
+        <v>682</v>
+      </c>
+      <c r="L21">
+        <v>3228</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1.6E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="D22">
-        <v>7.5999999999999998E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E22">
-        <v>0.29599999999999999</v>
+        <v>1.4E-2</v>
       </c>
       <c r="F22">
-        <v>1.804</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="G22">
-        <v>9.4879999999999995</v>
+        <v>0.434</v>
       </c>
       <c r="H22">
-        <v>56.268000000000001</v>
+        <v>2.7090000000000001</v>
+      </c>
+      <c r="I22">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J22">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C23">
-        <v>6.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D23">
-        <v>1.9E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E23">
-        <v>0.10100000000000001</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="F23">
-        <v>0.19600000000000001</v>
+        <v>1.804</v>
       </c>
       <c r="G23">
-        <v>0.63500000000000001</v>
+        <v>9.4879999999999995</v>
       </c>
       <c r="H23">
-        <v>3.383</v>
-      </c>
-      <c r="I23">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="J23">
-        <v>139</v>
+        <v>56.268000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0.65</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D24">
-        <v>3.5369999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E24">
-        <v>16.600000000000001</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F24">
-        <v>91</v>
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G24">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H24">
+        <v>3.383</v>
+      </c>
+      <c r="I24">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J24">
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0.16</v>
+      </c>
+      <c r="C25">
+        <v>0.65</v>
+      </c>
+      <c r="D25">
+        <v>3.5369999999999999</v>
+      </c>
+      <c r="E25">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.25800000000000001</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>1.25</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>6.2619999999999996</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>34.947000000000003</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>210.6</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>1352</v>
       </c>
     </row>

</xml_diff>